<commit_message>
Adicionando as histórias de usuário ao repositório.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Genérico/2-Gerencia de Projeto/Templates/Quadro de Gerenciamento de Risco (Scrum).xlsx
+++ b/Artefatos de Documentação/Processo Genérico/2-Gerencia de Projeto/Templates/Quadro de Gerenciamento de Risco (Scrum).xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="123820"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Dropbox\Engenharia de Software\5º Periodo\Trabalho Multidisciplinar\Repositório\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
@@ -18,7 +13,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="Acao">Valores!#REF!</definedName>
@@ -91,11 +85,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -783,64 +777,64 @@
     </xf>
   </cellXfs>
   <cellStyles count="58">
-    <cellStyle name="Accent1" xfId="1" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent1 - 20%" xfId="2"/>
     <cellStyle name="Accent1 - 20% 2" xfId="45"/>
     <cellStyle name="Accent1 - 40%" xfId="3"/>
     <cellStyle name="Accent1 - 40% 2" xfId="46"/>
     <cellStyle name="Accent1 - 60%" xfId="4"/>
-    <cellStyle name="Accent2" xfId="5" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 - 20%" xfId="6"/>
     <cellStyle name="Accent2 - 20% 2" xfId="47"/>
     <cellStyle name="Accent2 - 40%" xfId="7"/>
     <cellStyle name="Accent2 - 40% 2" xfId="48"/>
     <cellStyle name="Accent2 - 60%" xfId="8"/>
-    <cellStyle name="Accent3" xfId="9" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 - 20%" xfId="10"/>
     <cellStyle name="Accent3 - 20% 2" xfId="49"/>
     <cellStyle name="Accent3 - 40%" xfId="11"/>
     <cellStyle name="Accent3 - 40% 2" xfId="50"/>
     <cellStyle name="Accent3 - 60%" xfId="12"/>
-    <cellStyle name="Accent4" xfId="13" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 - 20%" xfId="14"/>
     <cellStyle name="Accent4 - 20% 2" xfId="51"/>
     <cellStyle name="Accent4 - 40%" xfId="15"/>
     <cellStyle name="Accent4 - 40% 2" xfId="52"/>
     <cellStyle name="Accent4 - 60%" xfId="16"/>
-    <cellStyle name="Accent5" xfId="17" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 - 20%" xfId="18"/>
     <cellStyle name="Accent5 - 20% 2" xfId="53"/>
     <cellStyle name="Accent5 - 40%" xfId="19"/>
     <cellStyle name="Accent5 - 40% 2" xfId="54"/>
     <cellStyle name="Accent5 - 60%" xfId="20"/>
-    <cellStyle name="Accent6" xfId="21" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 - 20%" xfId="22"/>
     <cellStyle name="Accent6 - 20% 2" xfId="55"/>
     <cellStyle name="Accent6 - 40%" xfId="23"/>
     <cellStyle name="Accent6 - 40% 2" xfId="56"/>
     <cellStyle name="Accent6 - 60%" xfId="24"/>
-    <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="31" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula de Verificação" xfId="27" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Célula Vinculada" xfId="37" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Emphasis 1" xfId="28"/>
     <cellStyle name="Emphasis 2" xfId="29"/>
     <cellStyle name="Emphasis 3" xfId="30"/>
-    <cellStyle name="Good" xfId="31" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="32" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="33" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="35" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="36" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="37" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="38" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Ênfase1" xfId="1" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Ênfase2" xfId="5" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Ênfase3" xfId="9" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Ênfase4" xfId="13" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Ênfase5" xfId="17" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Ênfase6" xfId="21" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="36" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorreto" xfId="25" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutra" xfId="38" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="44"/>
-    <cellStyle name="Note" xfId="39" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="40" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="39" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Percent 2" xfId="57"/>
+    <cellStyle name="Saída" xfId="40" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Sheet Title" xfId="41"/>
+    <cellStyle name="Texto de Aviso" xfId="43" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="32" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="33" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="34" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="35" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="80">
     <dxf>
@@ -1470,7 +1464,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instrucoes"/>
@@ -1567,35 +1561,10 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Instrucoes"/>
-      <sheetName val="Riscos"/>
-      <sheetName val="Issues"/>
-      <sheetName val="Acoes"/>
-      <sheetName val="Grafico"/>
-      <sheetName val="EAR"/>
-      <sheetName val="Param"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1633,9 +1602,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1667,10 +1636,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1702,10 +1670,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1875,14 +1842,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
@@ -1894,13 +1861,13 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7">
       <c r="B1" s="4"/>
       <c r="D1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="30">
       <c r="B2" s="18" t="s">
         <v>6</v>
       </c>
@@ -1920,7 +1887,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7">
       <c r="B3" s="20">
         <v>1</v>
       </c>
@@ -1933,7 +1900,7 @@
       <c r="F3" s="21"/>
       <c r="G3" s="20"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7">
       <c r="B4" s="21">
         <f>B3+1</f>
         <v>2</v>
@@ -1947,7 +1914,7 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" s="8" customFormat="1">
       <c r="B5" s="21">
         <f t="shared" ref="B5:B17" si="1">B4+1</f>
         <v>3</v>
@@ -1961,7 +1928,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" s="8" customFormat="1">
       <c r="B6" s="21">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1975,7 +1942,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" s="8" customFormat="1">
       <c r="B7" s="21">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1989,7 +1956,7 @@
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" s="8" customFormat="1">
       <c r="B8" s="21">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2003,7 +1970,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" s="8" customFormat="1">
       <c r="B9" s="21">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2017,7 +1984,7 @@
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" s="8" customFormat="1">
       <c r="B10" s="21">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -2031,7 +1998,7 @@
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" s="8" customFormat="1">
       <c r="B11" s="21">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2045,7 +2012,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" s="8" customFormat="1">
       <c r="B12" s="21">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2059,7 +2026,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" s="8" customFormat="1">
       <c r="B13" s="21">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2073,7 +2040,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" s="8" customFormat="1">
       <c r="B14" s="21">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2087,7 +2054,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" s="8" customFormat="1">
       <c r="B15" s="21">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2101,7 +2068,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" s="8" customFormat="1">
       <c r="B16" s="21">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2115,7 +2082,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" s="8" customFormat="1">
       <c r="B17" s="21">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2129,17 +2096,17 @@
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="C18" s="9"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7">
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7">
       <c r="B23" s="10"/>
     </row>
   </sheetData>
@@ -2403,29 +2370,27 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;LPlano de gerenciamento dos riscos&amp;R&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;F
-PMO Escritório de Projetos&amp;RPágina &amp;P de &amp;N
-http://escritoriodeprojetos.com.br</oddFooter>
+    <oddFooter>&amp;L&amp;FPMO Escritório de Projetos&amp;RPágina &amp;P de &amp;Nhttp://escritoriodeprojetos.com.br</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5">
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
@@ -2435,7 +2400,7 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" s="3">
         <f>B4+1</f>
         <v>3</v>
@@ -2453,7 +2418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" s="3">
         <f>B5+1</f>
         <v>2</v>
@@ -2471,7 +2436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -2488,7 +2453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2529,22 +2494,20 @@
   <pageSetup paperSize="65" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;LPlano de gerenciamento dos riscos&amp;R&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;F
-PMO Escritório de Projetos&amp;RPágina &amp;P de &amp;N
-http://escritoriodeprojetos.com.br</oddFooter>
+    <oddFooter>&amp;L&amp;FPMO Escritório de Projetos&amp;RPágina &amp;P de &amp;Nhttp://escritoriodeprojetos.com.br</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="X9" workbookViewId="0">
+      <selection activeCell="AQ33" sqref="AQ33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" style="1" customWidth="1"/>
@@ -2553,7 +2516,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="30">
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
@@ -2564,14 +2527,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4">
       <c r="B3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4">
       <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
@@ -2582,7 +2545,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4">
       <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
@@ -2593,7 +2556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4">
       <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
@@ -2604,14 +2567,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4">
       <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4">
       <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
@@ -2623,9 +2586,7 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;LPlano de gerenciamento dos riscos&amp;R&amp;A</oddHeader>
-    <oddFooter>&amp;L&amp;F
-PMO Escritório de Projetos&amp;RPágina &amp;P de &amp;N
-http://escritoriodeprojetos.com.br</oddFooter>
+    <oddFooter>&amp;L&amp;FPMO Escritório de Projetos&amp;RPágina &amp;P de &amp;Nhttp://escritoriodeprojetos.com.br</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revisão Geral no Processo de GRE.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Genérico/2-Gerencia de Projeto/Templates/Quadro de Gerenciamento de Risco (Scrum).xlsx
+++ b/Artefatos de Documentação/Processo Genérico/2-Gerencia de Projeto/Templates/Quadro de Gerenciamento de Risco (Scrum).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="123820"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\Dropbox\UFG\GitHubProjects\P.I.-ES-UFG-2015-BIJLMMV\Artefatos de Documentação\Processo Genérico\2-Gerencia de Projeto\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="4" r:id="rId1"/>
@@ -85,11 +90,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1464,7 +1469,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Instrucoes"/>
@@ -1604,7 +1609,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1636,9 +1641,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1670,6 +1676,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1842,18 +1849,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12" style="5" customWidth="1"/>
     <col min="4" max="4" width="29.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" style="5" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" style="5" customWidth="1"/>
@@ -1861,13 +1868,13 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="4"/>
       <c r="D1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="2:7" ht="30">
+    <row r="2" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>6</v>
       </c>
@@ -1887,20 +1894,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="20">
         <v>1</v>
       </c>
       <c r="C3" s="19">
         <f t="shared" ref="C3:C17" si="0">$E3+$F3</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="E3" s="21">
+        <v>1</v>
+      </c>
+      <c r="F3" s="21">
+        <v>1</v>
+      </c>
       <c r="G3" s="20"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="21">
         <f>B3+1</f>
         <v>2</v>
@@ -1914,7 +1925,7 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="2:7" s="8" customFormat="1">
+    <row r="5" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="21">
         <f t="shared" ref="B5:B17" si="1">B4+1</f>
         <v>3</v>
@@ -1928,7 +1939,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="2:7" s="8" customFormat="1">
+    <row r="6" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="21">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1942,7 +1953,7 @@
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="2:7" s="8" customFormat="1">
+    <row r="7" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="21">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1956,7 +1967,7 @@
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="2:7" s="8" customFormat="1">
+    <row r="8" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="21">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1970,7 +1981,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="2:7" s="8" customFormat="1">
+    <row r="9" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="21">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1984,7 +1995,7 @@
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="2:7" s="8" customFormat="1">
+    <row r="10" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="21">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1998,7 +2009,7 @@
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="2:7" s="8" customFormat="1">
+    <row r="11" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="21">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2012,7 +2023,7 @@
       <c r="F11" s="21"/>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="2:7" s="8" customFormat="1">
+    <row r="12" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="21">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2026,7 +2037,7 @@
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="2:7" s="8" customFormat="1">
+    <row r="13" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="21">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2040,7 +2051,7 @@
       <c r="F13" s="21"/>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="2:7" s="8" customFormat="1">
+    <row r="14" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="21">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2054,7 +2065,7 @@
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
     </row>
-    <row r="15" spans="2:7" s="8" customFormat="1">
+    <row r="15" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="21">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2068,7 +2079,7 @@
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
     </row>
-    <row r="16" spans="2:7" s="8" customFormat="1">
+    <row r="16" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="21">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2082,7 +2093,7 @@
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="2:7" s="8" customFormat="1">
+    <row r="17" spans="2:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="21">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2096,17 +2107,17 @@
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C18" s="9"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
     </row>
   </sheetData>
@@ -2376,21 +2387,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
@@ -2400,7 +2411,7 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <f>B4+1</f>
         <v>3</v>
@@ -2418,7 +2429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <f>B5+1</f>
         <v>2</v>
@@ -2436,7 +2447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -2453,7 +2464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2500,14 +2511,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="X9" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="X9" workbookViewId="0">
       <selection activeCell="AQ33" sqref="AQ33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" style="1" customWidth="1"/>
@@ -2516,7 +2527,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="30">
+    <row r="2" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
@@ -2527,14 +2538,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
@@ -2545,7 +2556,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>10</v>
       </c>
@@ -2556,7 +2567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
@@ -2567,14 +2578,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>13</v>
       </c>

</xml_diff>